<commit_message>
Doing Week1 Lesson4 Postclass
</commit_message>
<xml_diff>
--- a/SA 1/Week1/L4/01_04_Absolute_Relative.xlsx
+++ b/SA 1/Week1/L4/01_04_Absolute_Relative.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitRepo\MUFYICT\SA 1\Week1\L4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepo\MUFYICT\SA 1\Week1\L4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16457" windowHeight="5546"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16455" windowHeight="5550" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="relative" sheetId="1" r:id="rId1"/>
@@ -337,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -361,6 +361,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1368,18 +1369,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6:Q6"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="5.69140625" customWidth="1"/>
-    <col min="10" max="10" width="12.3828125" customWidth="1"/>
-    <col min="18" max="18" width="5.3046875" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" customWidth="1"/>
+    <col min="18" max="18" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:19" ht="29.15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1417,7 +1418,7 @@
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
     </row>
-    <row r="4" spans="1:19" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1459,7 +1460,7 @@
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
     </row>
-    <row r="5" spans="1:19" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1501,7 +1502,7 @@
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
     </row>
-    <row r="6" spans="1:19" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -1549,7 +1550,7 @@
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
     </row>
-    <row r="7" spans="1:19" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1574,7 +1575,7 @@
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
     </row>
-    <row r="8" spans="1:19" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1599,7 +1600,7 @@
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
     </row>
-    <row r="9" spans="1:19" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -1614,7 +1615,7 @@
         <v>6.8310000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -1629,7 +1630,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -1644,7 +1645,7 @@
         <v>7.4750000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -1660,6 +1661,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1670,17 +1672,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C15" activeCellId="1" sqref="D3:D8 C15:G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="7" t="s">
         <v>20</v>
@@ -1700,75 +1702,93 @@
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="1:10" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="3">
         <v>38</v>
       </c>
-      <c r="D3" s="11"/>
+      <c r="D3" s="11">
+        <f>C3*$E$3</f>
+        <v>931</v>
+      </c>
       <c r="E3" s="8">
         <v>24.5</v>
       </c>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="3">
         <v>24</v>
       </c>
-      <c r="D4" s="11"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="D4" s="11">
+        <f t="shared" ref="D4:D8" si="0">C4*$E$3</f>
+        <v>588</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="3">
         <v>40</v>
       </c>
-      <c r="D5" s="11"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="D5" s="11">
+        <f t="shared" si="0"/>
+        <v>980</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C6" s="3">
         <v>30</v>
       </c>
-      <c r="D6" s="11"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="D6" s="11">
+        <f t="shared" si="0"/>
+        <v>735</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="3">
         <v>22</v>
       </c>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="D7" s="11">
+        <f t="shared" si="0"/>
+        <v>539</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="3">
         <v>8</v>
       </c>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="D8" s="11">
+        <f t="shared" si="0"/>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:10" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
         <v>29</v>
       </c>
@@ -1780,7 +1800,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:10" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
         <v>30</v>
       </c>
@@ -1800,7 +1820,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
         <v>36</v>
       </c>
@@ -1820,17 +1840,33 @@
         <v>3.4500000000000003E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="C15" s="5">
+        <f>C14*$C$12</f>
+        <v>395</v>
+      </c>
+      <c r="D15" s="5">
+        <f t="shared" ref="D15:G15" si="1">D14*$C$12</f>
+        <v>405</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="F15" s="5">
+        <f t="shared" si="1"/>
+        <v>295</v>
+      </c>
+      <c r="G15" s="5">
+        <f t="shared" si="1"/>
+        <v>345.00000000000006</v>
+      </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1840,26 +1876,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="12" max="12" width="13.69140625" customWidth="1"/>
+    <col min="1" max="1" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1894,7 +1934,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -1916,10 +1956,16 @@
       <c r="G7" s="8">
         <v>260</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="H7" s="17">
+        <f>SUM(D7:G7)</f>
+        <v>1057</v>
+      </c>
+      <c r="I7" s="13">
+        <f>H7*$M$6</f>
+        <v>105.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -1941,10 +1987,16 @@
       <c r="G8" s="8">
         <v>485</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="H8" s="17">
+        <f t="shared" ref="H8:H16" si="0">SUM(D8:G8)</f>
+        <v>1057</v>
+      </c>
+      <c r="I8" s="13">
+        <f t="shared" ref="I8:I16" si="1">H8*$M$6</f>
+        <v>105.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -1966,10 +2018,16 @@
       <c r="G9" s="8">
         <v>960</v>
       </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="H9" s="17">
+        <f t="shared" si="0"/>
+        <v>3067</v>
+      </c>
+      <c r="I9" s="13">
+        <f t="shared" si="1"/>
+        <v>306.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -1991,10 +2049,16 @@
       <c r="G10" s="8">
         <v>406</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="H10" s="17">
+        <f t="shared" si="0"/>
+        <v>1808</v>
+      </c>
+      <c r="I10" s="13">
+        <f t="shared" si="1"/>
+        <v>180.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -2016,10 +2080,16 @@
       <c r="G11" s="8">
         <v>581</v>
       </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="H11" s="17">
+        <f t="shared" si="0"/>
+        <v>1439</v>
+      </c>
+      <c r="I11" s="13">
+        <f t="shared" si="1"/>
+        <v>143.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -2041,10 +2111,16 @@
       <c r="G12" s="8">
         <v>636</v>
       </c>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="H12" s="17">
+        <f t="shared" si="0"/>
+        <v>1718</v>
+      </c>
+      <c r="I12" s="13">
+        <f t="shared" si="1"/>
+        <v>171.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -2066,10 +2142,16 @@
       <c r="G13" s="8">
         <v>625</v>
       </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="H13" s="17">
+        <f t="shared" si="0"/>
+        <v>2528</v>
+      </c>
+      <c r="I13" s="13">
+        <f t="shared" si="1"/>
+        <v>252.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>66</v>
       </c>
@@ -2091,10 +2173,16 @@
       <c r="G14" s="8">
         <v>356</v>
       </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="H14" s="17">
+        <f t="shared" si="0"/>
+        <v>1294</v>
+      </c>
+      <c r="I14" s="13">
+        <f t="shared" si="1"/>
+        <v>129.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -2116,10 +2204,16 @@
       <c r="G15" s="8">
         <v>398</v>
       </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="H15" s="17">
+        <f t="shared" si="0"/>
+        <v>1891</v>
+      </c>
+      <c r="I15" s="13">
+        <f t="shared" si="1"/>
+        <v>189.10000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -2141,63 +2235,231 @@
       <c r="G16" s="8">
         <v>489</v>
       </c>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H16" s="17">
+        <f t="shared" si="0"/>
+        <v>2383</v>
+      </c>
+      <c r="I16" s="13">
+        <f t="shared" si="1"/>
+        <v>238.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>75</v>
       </c>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="17">
+        <f>SUM(D7:D16)</f>
+        <v>4668</v>
+      </c>
+      <c r="E17" s="17">
+        <f t="shared" ref="E17:G17" si="2">SUM(E7:E16)</f>
+        <v>4687</v>
+      </c>
+      <c r="F17" s="17">
+        <f t="shared" si="2"/>
+        <v>3691</v>
+      </c>
+      <c r="G17" s="17">
+        <f t="shared" si="2"/>
+        <v>5196</v>
+      </c>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>72</v>
       </c>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="17">
+        <f>AVERAGE(D7:D16)</f>
+        <v>466.8</v>
+      </c>
+      <c r="E18" s="17">
+        <f t="shared" ref="E18:G18" si="3">AVERAGE(E7:E16)</f>
+        <v>468.7</v>
+      </c>
+      <c r="F18" s="17">
+        <f t="shared" si="3"/>
+        <v>369.1</v>
+      </c>
+      <c r="G18" s="17">
+        <f t="shared" si="3"/>
+        <v>519.6</v>
+      </c>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>73</v>
       </c>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="D19" s="17">
+        <f>MIN(D7:D16)</f>
+        <v>88</v>
+      </c>
+      <c r="E19" s="17">
+        <f t="shared" ref="E19:G19" si="4">MIN(E7:E16)</f>
+        <v>146</v>
+      </c>
+      <c r="F19" s="17">
+        <f t="shared" si="4"/>
+        <v>127</v>
+      </c>
+      <c r="G19" s="17">
+        <f t="shared" si="4"/>
+        <v>260</v>
+      </c>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>74</v>
       </c>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="D20" s="17">
+        <f>MAX(D7:D16)</f>
+        <v>895</v>
+      </c>
+      <c r="E20" s="17">
+        <f t="shared" ref="E20:G20" si="5">MAX(E7:E16)</f>
+        <v>758</v>
+      </c>
+      <c r="F20" s="17">
+        <f t="shared" si="5"/>
+        <v>819</v>
+      </c>
+      <c r="G20" s="17">
+        <f t="shared" si="5"/>
+        <v>960</v>
+      </c>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D7:G16">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5A4E9E94-B2E5-4A49-B59A-6CB6CF581A7A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7:I16">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2835041C-26F9-45E8-86FC-2B5B31D6C0CC}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:G20">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{7BD171C8-B273-4905-97CE-BDF469FE33BB}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{BF057FD4-A24B-4877-9390-F69A96F1C71E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5A4E9E94-B2E5-4A49-B59A-6CB6CF581A7A}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D7:G16</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2835041C-26F9-45E8-86FC-2B5B31D6C0CC}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D7:I16</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{7BD171C8-B273-4905-97CE-BDF469FE33BB}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D10:G20</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{BF057FD4-A24B-4877-9390-F69A96F1C71E}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>A1:XFD1048576</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>